<commit_message>
corrections erreurs build et création table de bd
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="4890"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table7" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -377,7 +377,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
retiré fonctions deprecated de apache POI
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="4890"/>
   </bookViews>
   <sheets>
-    <sheet name="Table7" sheetId="1" r:id="rId1"/>
+    <sheet name="Table8" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -377,7 +377,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
first main class refactor in classes
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="4890"/>
   </bookViews>
   <sheets>
-    <sheet name="Table8" sheetId="1" r:id="rId1"/>
+    <sheet name="Table12" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -377,7 +377,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added smtg to show new table (not yet working)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="13335" windowHeight="4890"/>
   </bookViews>
   <sheets>
-    <sheet name="Table12" sheetId="1" r:id="rId1"/>
+    <sheet name="Table19" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -18,15 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>EmployeeNumber</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>André</t>
   </si>
   <si>
@@ -43,6 +34,15 @@
   </si>
   <si>
     <t>Carmant</t>
+  </si>
+  <si>
+    <t>employeenumber</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
   </si>
 </sst>
 </file>
@@ -377,23 +377,25 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -401,10 +403,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -412,10 +414,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -423,10 +425,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retrieve + insert + query qui marchent!!!
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>André</t>
-  </si>
-  <si>
     <t>Belmont</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>lastname</t>
+  </si>
+  <si>
+    <t>Andre</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -389,13 +389,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -403,10 +403,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -414,10 +414,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -425,10 +425,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Readme update and minor formatting changes
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_file/EmployeeData.xlsx
+++ b/src/main/resources/excel_file/EmployeeData.xlsx
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Belmont</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Tanguay</t>
-  </si>
-  <si>
-    <t>Carl</t>
-  </si>
-  <si>
-    <t>Carmant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>employeenumber</t>
   </si>
@@ -42,7 +27,40 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>Andre</t>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Comtois</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>Paré</t>
+  </si>
+  <si>
+    <t>Jean-Michel</t>
+  </si>
+  <si>
+    <t>Esquive</t>
+  </si>
+  <si>
+    <t>Thierry</t>
+  </si>
+  <si>
+    <t>Plinplinplon</t>
+  </si>
+  <si>
+    <t>Agzend</t>
+  </si>
+  <si>
+    <t>Fireman</t>
+  </si>
+  <si>
+    <t>Jean-Claude</t>
+  </si>
+  <si>
+    <t>Van Damme</t>
   </si>
 </sst>
 </file>
@@ -374,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -389,46 +407,79 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>